<commit_message>
Begin hand conversion of old data formats to new reference format
</commit_message>
<xml_diff>
--- a/inst/FloridaPhase2_datasheet.xlsx
+++ b/inst/FloridaPhase2_datasheet.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="dust_table_1.1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -403,7 +403,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +539,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -837,7 +853,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -880,11 +896,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -913,11 +933,15 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1265,10 +1289,13 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -1942,6 +1969,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>